<commit_message>
Add the Class and rest.
</commit_message>
<xml_diff>
--- a/quronghui_Table/Class and rest.xlsx
+++ b/quronghui_Table/Class and rest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2018_Hardware_Files\quronghui_Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HUST_Files\2018-Hust-Hardware-FIles\quronghui_Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37A47F4-90FC-4D86-B815-EAA072541C4C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="课程时间表" sheetId="1" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="201">
   <si>
     <t>一</t>
   </si>
@@ -921,12 +920,58 @@
     <t>提供两种方式：C51和买了MPU6000</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>看了一点，开了一上午的会</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找了ADS1299和OPENBCI的区别</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成情况 √  ×</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有进行查找</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找了ADS1299和OPENBCI的区别，重新绘制原理图</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有进行</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> ×</t>
+  </si>
+  <si>
+    <t>没有上课，绘制SCH的原理图</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>绘制SCH的原理图</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> √</t>
+  </si>
+  <si>
+    <t>没有上课</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <name val="等线"/>
@@ -1123,7 +1168,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1223,6 +1268,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1233,53 +1296,41 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1287,6 +1338,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1568,14 +1622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="40" workbookViewId="0">
       <selection activeCell="E10" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="20" customWidth="1"/>
@@ -1591,23 +1645,23 @@
     <col min="258" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:13" ht="42" customHeight="1">
+      <c r="B1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
       <c r="M1" s="21"/>
     </row>
-    <row r="2" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" ht="20.25" customHeight="1">
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -1622,16 +1676,16 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="36"/>
-    </row>
-    <row r="3" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="M2" s="35"/>
+    </row>
+    <row r="3" spans="2:13" ht="29.25" customHeight="1">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
         <v>0</v>
@@ -1654,14 +1708,14 @@
       <c r="K3" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-    </row>
-    <row r="4" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+    </row>
+    <row r="4" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -1688,12 +1742,12 @@
       <c r="K4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="L4" s="40"/>
-      <c r="M4" s="41"/>
-    </row>
-    <row r="5" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="39"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="43"/>
+    </row>
+    <row r="5" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
@@ -1718,12 +1772,12 @@
       <c r="K5" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-    </row>
-    <row r="6" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
-      <c r="C6" s="39"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+    </row>
+    <row r="6" spans="2:13" ht="24.75" customHeight="1">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="21" t="s">
         <v>6</v>
       </c>
@@ -1748,11 +1802,11 @@
       <c r="K6" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-    </row>
-    <row r="7" spans="2:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+    </row>
+    <row r="7" spans="2:13" ht="24.75" customHeight="1">
+      <c r="B7" s="35"/>
       <c r="C7" s="27" t="s">
         <v>114</v>
       </c>
@@ -1770,12 +1824,12 @@
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-    </row>
-    <row r="8" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+    </row>
+    <row r="8" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="38" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -1802,12 +1856,12 @@
       <c r="K8" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-    </row>
-    <row r="9" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+    </row>
+    <row r="9" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="21" t="s">
         <v>5</v>
       </c>
@@ -1830,12 +1884,12 @@
       <c r="K9" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-    </row>
-    <row r="10" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+    </row>
+    <row r="10" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="21" t="s">
         <v>6</v>
       </c>
@@ -1854,10 +1908,10 @@
       </c>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-    </row>
-    <row r="11" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+    </row>
+    <row r="11" spans="2:13" ht="13.5" customHeight="1">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -1871,8 +1925,8 @@
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
     </row>
-    <row r="12" spans="2:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="12" spans="2:13" ht="33.75" customHeight="1">
+      <c r="B12" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -1897,8 +1951,8 @@
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
     </row>
-    <row r="13" spans="2:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="36"/>
+    <row r="13" spans="2:13" ht="33.75" customHeight="1">
+      <c r="B13" s="35"/>
       <c r="C13" s="21" t="s">
         <v>59</v>
       </c>
@@ -1919,7 +1973,7 @@
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
     </row>
-    <row r="14" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" ht="12.75" customHeight="1">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -1933,11 +1987,11 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
     </row>
-    <row r="15" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="38" t="s">
         <v>142</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -1964,12 +2018,12 @@
       <c r="K15" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-    </row>
-    <row r="16" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+    </row>
+    <row r="16" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="21" t="s">
         <v>5</v>
       </c>
@@ -1994,12 +2048,12 @@
       <c r="K16" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-    </row>
-    <row r="17" spans="2:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+    </row>
+    <row r="17" spans="2:13" ht="32.25" customHeight="1">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
@@ -2020,12 +2074,12 @@
         <v>123</v>
       </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-    </row>
-    <row r="18" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37" t="s">
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+    </row>
+    <row r="18" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B18" s="35"/>
+      <c r="C18" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -2046,12 +2100,12 @@
         <v>125</v>
       </c>
       <c r="K18" s="21"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-    </row>
-    <row r="19" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+    </row>
+    <row r="19" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="21" t="s">
         <v>5</v>
       </c>
@@ -2068,12 +2122,12 @@
       </c>
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-    </row>
-    <row r="20" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+    </row>
+    <row r="20" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="21" t="s">
         <v>6</v>
       </c>
@@ -2088,10 +2142,10 @@
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-    </row>
-    <row r="21" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+    </row>
+    <row r="21" spans="2:13" ht="11.25" customHeight="1">
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -2105,7 +2159,7 @@
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
     </row>
-    <row r="22" spans="2:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" ht="27.75" customHeight="1">
       <c r="B22" s="21" t="s">
         <v>45</v>
       </c>
@@ -2127,7 +2181,7 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
     </row>
-    <row r="23" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" ht="13.5" customHeight="1">
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -2141,11 +2195,11 @@
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
     </row>
-    <row r="24" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -2172,12 +2226,12 @@
       <c r="K24" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="21" t="s">
         <v>5</v>
       </c>
@@ -2200,12 +2254,12 @@
       <c r="K25" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-    </row>
-    <row r="26" spans="2:13" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+    </row>
+    <row r="26" spans="2:13" ht="19.149999999999999" customHeight="1">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="21" t="s">
         <v>6</v>
       </c>
@@ -2222,12 +2276,12 @@
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-    </row>
-    <row r="27" spans="2:13" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="36"/>
-      <c r="C27" s="38" t="s">
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+    </row>
+    <row r="27" spans="2:13" ht="23.85" customHeight="1">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -2252,12 +2306,12 @@
       <c r="K27" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-    </row>
-    <row r="28" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36"/>
-      <c r="C28" s="39"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+    </row>
+    <row r="28" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="21" t="s">
         <v>5</v>
       </c>
@@ -2278,12 +2332,12 @@
       <c r="K28" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-    </row>
-    <row r="29" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+    </row>
+    <row r="29" spans="2:13" ht="24.95" customHeight="1">
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="25" t="s">
@@ -2298,12 +2352,12 @@
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
       <c r="K29" s="21"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
-      <c r="C30" s="39"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="B30" s="35"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="21" t="s">
         <v>6</v>
       </c>
@@ -2318,19 +2372,12 @@
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
       <c r="K30" s="21"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-    </row>
-    <row r="36" ht="87.2" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+    </row>
+    <row r="36" ht="87.2" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L24:M30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C24:C26"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B15:B20"/>
@@ -2341,6 +2388,13 @@
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="L4:M10"/>
+    <mergeCell ref="L24:M30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C24:C26"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2349,14 +2403,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IT36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="1" customWidth="1"/>
@@ -2371,20 +2425,20 @@
     <col min="11" max="254" width="9" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="2:10" ht="42" customHeight="1">
+      <c r="B1" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-    </row>
-    <row r="2" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+    </row>
+    <row r="2" spans="2:10" ht="20.25" customHeight="1">
       <c r="B2" s="2"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2395,11 +2449,11 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="2:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+    <row r="3" spans="2:10" ht="29.25" customHeight="1">
+      <c r="B3" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="51"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="2"/>
       <c r="E3" s="24" t="s">
         <v>0</v>
@@ -2416,11 +2470,11 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="43" t="s">
+    <row r="4" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B4" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="49" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -2437,9 +2491,9 @@
       <c r="I4" s="2"/>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43"/>
-      <c r="C5" s="47"/>
+    <row r="5" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B5" s="48"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2454,9 +2508,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="43"/>
-      <c r="C6" s="47"/>
+    <row r="6" spans="2:10" ht="24.75" customHeight="1">
+      <c r="B6" s="48"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2471,8 +2525,8 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="43"/>
+    <row r="7" spans="2:10" ht="24.75" customHeight="1">
+      <c r="B7" s="48"/>
       <c r="C7" s="15" t="s">
         <v>114</v>
       </c>
@@ -2490,9 +2544,9 @@
       <c r="I7" s="12"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="43"/>
-      <c r="C8" s="44" t="s">
+    <row r="8" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B8" s="48"/>
+      <c r="C8" s="51" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -2507,9 +2561,9 @@
       <c r="I8" s="16"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+    <row r="9" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2522,9 +2576,9 @@
       <c r="I9" s="13"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
+    <row r="10" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
@@ -2537,7 +2591,7 @@
       <c r="I10" s="13"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="13.5" customHeight="1">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2548,8 +2602,8 @@
       <c r="I11" s="13"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="42" t="s">
+    <row r="12" spans="2:10" ht="33.75" customHeight="1">
+      <c r="B12" s="52" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2569,8 +2623,8 @@
       <c r="I12" s="12"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="42"/>
+    <row r="13" spans="2:10" ht="33.75" customHeight="1">
+      <c r="B13" s="52"/>
       <c r="C13" s="12" t="s">
         <v>59</v>
       </c>
@@ -2588,7 +2642,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="12.75" customHeight="1">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -2599,11 +2653,11 @@
       <c r="I14" s="12"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="43" t="s">
+    <row r="15" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B15" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="51" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2618,9 +2672,9 @@
       <c r="I15" s="13"/>
       <c r="J15" s="14"/>
     </row>
-    <row r="16" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
+    <row r="16" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="2" t="s">
         <v>5</v>
       </c>
@@ -2633,9 +2687,9 @@
       <c r="I16" s="13"/>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+    <row r="17" spans="2:10" ht="32.25" customHeight="1">
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
@@ -2648,9 +2702,9 @@
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="43"/>
-      <c r="C18" s="44" t="s">
+    <row r="18" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B18" s="48"/>
+      <c r="C18" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -2669,9 +2723,9 @@
       <c r="I18" s="13"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
+    <row r="19" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
@@ -2684,9 +2738,9 @@
       <c r="I19" s="13"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+    <row r="20" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
@@ -2699,7 +2753,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" ht="11.25" customHeight="1">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2710,7 +2764,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" ht="27.75" customHeight="1">
       <c r="B22" s="12" t="s">
         <v>45</v>
       </c>
@@ -2727,7 +2781,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" ht="13.5" customHeight="1">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="2"/>
@@ -2738,11 +2792,11 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="43" t="s">
+    <row r="24" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B24" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="53" t="s">
         <v>76</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -2761,9 +2815,9 @@
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
+    <row r="25" spans="2:10">
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="2" t="s">
         <v>5</v>
       </c>
@@ -2776,9 +2830,9 @@
       <c r="I25" s="2"/>
       <c r="J25" s="13"/>
     </row>
-    <row r="26" spans="2:10" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
+    <row r="26" spans="2:10" ht="19.149999999999999" customHeight="1">
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
       <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
@@ -2795,9 +2849,9 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="43"/>
-      <c r="C27" s="46" t="s">
+    <row r="27" spans="2:10" ht="23.85" customHeight="1">
+      <c r="B27" s="48"/>
+      <c r="C27" s="49" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -2816,9 +2870,9 @@
       <c r="I27" s="2"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="43"/>
-      <c r="C28" s="47"/>
+    <row r="28" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B28" s="48"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="2" t="s">
         <v>5</v>
       </c>
@@ -2829,9 +2883,9 @@
       <c r="I28" s="2"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="43"/>
-      <c r="C29" s="47"/>
+    <row r="29" spans="2:10" ht="24.95" customHeight="1">
+      <c r="B29" s="48"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="2"/>
       <c r="E29" s="24"/>
       <c r="F29" s="13"/>
@@ -2840,9 +2894,9 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="43"/>
-      <c r="C30" s="47"/>
+    <row r="30" spans="2:10">
+      <c r="B30" s="48"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="2" t="s">
         <v>6</v>
       </c>
@@ -2853,14 +2907,9 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="36" ht="87.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="87.2" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="C15:C17"/>
@@ -2868,6 +2917,11 @@
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2875,14 +2929,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV36"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="20" customWidth="1"/>
@@ -2897,22 +2951,22 @@
     <col min="257" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:12" ht="42" customHeight="1">
+      <c r="B1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" ht="20.25" customHeight="1">
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -2922,14 +2976,14 @@
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-    </row>
-    <row r="3" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+    </row>
+    <row r="3" spans="2:12" ht="29.25" customHeight="1">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
         <v>1</v>
@@ -2945,14 +2999,14 @@
       </c>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-    </row>
-    <row r="4" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+    </row>
+    <row r="4" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -2972,12 +3026,12 @@
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="41"/>
-    </row>
-    <row r="5" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="39"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
+    </row>
+    <row r="5" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
@@ -2993,12 +3047,12 @@
       </c>
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-    </row>
-    <row r="6" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
-      <c r="C6" s="39"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+    </row>
+    <row r="6" spans="2:12" ht="24.75" customHeight="1">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="21" t="s">
         <v>6</v>
       </c>
@@ -3010,11 +3064,11 @@
       <c r="H6" s="13"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-    </row>
-    <row r="7" spans="2:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+    </row>
+    <row r="7" spans="2:12" ht="24.75" customHeight="1">
+      <c r="B7" s="35"/>
       <c r="C7" s="27" t="s">
         <v>114</v>
       </c>
@@ -3031,12 +3085,12 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-    </row>
-    <row r="8" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="38" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -3050,12 +3104,12 @@
       <c r="H8" s="16"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-    </row>
-    <row r="9" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+    </row>
+    <row r="9" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="21" t="s">
         <v>5</v>
       </c>
@@ -3065,12 +3119,12 @@
       <c r="H9" s="25"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-    </row>
-    <row r="10" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+    </row>
+    <row r="10" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="21" t="s">
         <v>6</v>
       </c>
@@ -3080,10 +3134,10 @@
       <c r="H10" s="25"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-    </row>
-    <row r="11" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+    </row>
+    <row r="11" spans="2:12" ht="13.5" customHeight="1">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -3096,8 +3150,8 @@
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
     </row>
-    <row r="12" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="12" spans="2:12" ht="33.75" customHeight="1">
+      <c r="B12" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -3115,8 +3169,8 @@
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="36"/>
+    <row r="13" spans="2:12" ht="33.75" customHeight="1">
+      <c r="B13" s="35"/>
       <c r="C13" s="21" t="s">
         <v>59</v>
       </c>
@@ -3132,7 +3186,7 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" ht="12.75" customHeight="1">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -3145,11 +3199,11 @@
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="38" t="s">
         <v>142</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -3167,12 +3221,12 @@
       </c>
       <c r="I15" s="26"/>
       <c r="J15" s="26"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-    </row>
-    <row r="16" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+    </row>
+    <row r="16" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="21" t="s">
         <v>5</v>
       </c>
@@ -3184,12 +3238,12 @@
       <c r="H16" s="25"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-    </row>
-    <row r="17" spans="2:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+    </row>
+    <row r="17" spans="2:12" ht="32.25" customHeight="1">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
@@ -3203,12 +3257,12 @@
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-    </row>
-    <row r="18" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37" t="s">
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+    </row>
+    <row r="18" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B18" s="35"/>
+      <c r="C18" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -3220,12 +3274,12 @@
       <c r="H18" s="25"/>
       <c r="I18" s="21"/>
       <c r="J18" s="21"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-    </row>
-    <row r="19" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="21" t="s">
         <v>5</v>
       </c>
@@ -3235,12 +3289,12 @@
       <c r="H19" s="25"/>
       <c r="I19" s="21"/>
       <c r="J19" s="21"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-    </row>
-    <row r="20" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="21" t="s">
         <v>6</v>
       </c>
@@ -3250,10 +3304,10 @@
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-    </row>
-    <row r="21" spans="2:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+    </row>
+    <row r="21" spans="2:12" ht="11.25" customHeight="1">
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -3266,7 +3320,7 @@
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
     </row>
-    <row r="22" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="27.75" customHeight="1">
       <c r="B22" s="21" t="s">
         <v>45</v>
       </c>
@@ -3283,7 +3337,7 @@
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
     </row>
-    <row r="23" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" ht="13.5" customHeight="1">
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -3296,11 +3350,11 @@
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
     </row>
-    <row r="24" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -3314,12 +3368,12 @@
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="21" t="s">
         <v>5</v>
       </c>
@@ -3331,12 +3385,12 @@
       <c r="H25" s="21"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-    </row>
-    <row r="26" spans="2:12" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+    </row>
+    <row r="26" spans="2:12" ht="19.149999999999999" customHeight="1">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="21" t="s">
         <v>6</v>
       </c>
@@ -3348,12 +3402,12 @@
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-    </row>
-    <row r="27" spans="2:12" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="36"/>
-      <c r="C27" s="38" t="s">
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+    </row>
+    <row r="27" spans="2:12" ht="23.85" customHeight="1">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -3371,12 +3425,12 @@
       </c>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-    </row>
-    <row r="28" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36"/>
-      <c r="C28" s="39"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+    </row>
+    <row r="28" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="21" t="s">
         <v>5</v>
       </c>
@@ -3388,12 +3442,12 @@
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-    </row>
-    <row r="29" spans="2:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+    </row>
+    <row r="29" spans="2:12" ht="24.95" customHeight="1">
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21"/>
       <c r="E29" s="25" t="s">
         <v>91</v>
@@ -3407,12 +3461,12 @@
       </c>
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
-      <c r="C30" s="39"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="35"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="21" t="s">
         <v>6</v>
       </c>
@@ -3424,20 +3478,12 @@
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-    </row>
-    <row r="36" ht="87.2" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+    </row>
+    <row r="36" ht="87.2" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="K4:L10"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="K24:L30"/>
@@ -3447,6 +3493,14 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="K15:L20"/>
     <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="K4:L10"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3455,14 +3509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="20" customWidth="1"/>
@@ -3476,21 +3530,21 @@
     <col min="256" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:11" ht="42" customHeight="1">
+      <c r="B1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" ht="20.25" customHeight="1">
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -3499,14 +3553,14 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-    </row>
-    <row r="3" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+    </row>
+    <row r="3" spans="2:11" ht="29.25" customHeight="1">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
         <v>2</v>
@@ -3521,14 +3575,14 @@
         <v>154</v>
       </c>
       <c r="I3" s="21"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-    </row>
-    <row r="4" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+    </row>
+    <row r="4" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -3543,12 +3597,12 @@
       <c r="G4" s="2"/>
       <c r="H4" s="13"/>
       <c r="I4" s="21"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="41"/>
-    </row>
-    <row r="5" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="39"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="43"/>
+    </row>
+    <row r="5" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
@@ -3561,12 +3615,12 @@
       <c r="G5" s="2"/>
       <c r="H5" s="13"/>
       <c r="I5" s="26"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-    </row>
-    <row r="6" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
-      <c r="C6" s="39"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+    </row>
+    <row r="6" spans="2:11" ht="24.75" customHeight="1">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="21" t="s">
         <v>6</v>
       </c>
@@ -3579,11 +3633,11 @@
       <c r="G6" s="2"/>
       <c r="H6" s="13"/>
       <c r="I6" s="21"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-    </row>
-    <row r="7" spans="2:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+    </row>
+    <row r="7" spans="2:11" ht="24.75" customHeight="1">
+      <c r="B7" s="35"/>
       <c r="C7" s="27" t="s">
         <v>114</v>
       </c>
@@ -3601,12 +3655,12 @@
         <v>186</v>
       </c>
       <c r="I7" s="21"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-    </row>
-    <row r="8" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+    </row>
+    <row r="8" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="38" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -3619,12 +3673,12 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="25"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-    </row>
-    <row r="9" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+    </row>
+    <row r="9" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="21" t="s">
         <v>5</v>
       </c>
@@ -3635,12 +3689,12 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="21"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-    </row>
-    <row r="10" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+    </row>
+    <row r="10" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="21" t="s">
         <v>6</v>
       </c>
@@ -3651,10 +3705,10 @@
       <c r="G10" s="2"/>
       <c r="H10" s="12"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-    </row>
-    <row r="11" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+    </row>
+    <row r="11" spans="2:11" ht="13.5" customHeight="1">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -3666,8 +3720,8 @@
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="12" spans="2:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="12" spans="2:11" ht="33.75" customHeight="1">
+      <c r="B12" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -3688,8 +3742,8 @@
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="2:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="36"/>
+    <row r="13" spans="2:11" ht="33.75" customHeight="1">
+      <c r="B13" s="35"/>
       <c r="C13" s="21" t="s">
         <v>59</v>
       </c>
@@ -3708,7 +3762,7 @@
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
     </row>
-    <row r="14" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" ht="12.75" customHeight="1">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -3720,11 +3774,11 @@
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="38" t="s">
         <v>142</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -3741,12 +3795,12 @@
         <v>187</v>
       </c>
       <c r="I15" s="26"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-    </row>
-    <row r="16" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+    </row>
+    <row r="16" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="21" t="s">
         <v>5</v>
       </c>
@@ -3757,12 +3811,12 @@
       <c r="G16" s="25"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-    </row>
-    <row r="17" spans="2:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+    </row>
+    <row r="17" spans="2:11" ht="32.25" customHeight="1">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
@@ -3771,12 +3825,12 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-    </row>
-    <row r="18" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37" t="s">
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+    </row>
+    <row r="18" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B18" s="35"/>
+      <c r="C18" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -3789,12 +3843,12 @@
       <c r="G18" s="25"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-    </row>
-    <row r="19" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+    </row>
+    <row r="19" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="21" t="s">
         <v>5</v>
       </c>
@@ -3805,12 +3859,12 @@
       <c r="G19" s="25"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-    </row>
-    <row r="20" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+    </row>
+    <row r="20" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="21" t="s">
         <v>6</v>
       </c>
@@ -3821,10 +3875,10 @@
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-    </row>
-    <row r="21" spans="2:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+    </row>
+    <row r="21" spans="2:11" ht="11.25" customHeight="1">
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -3836,7 +3890,7 @@
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="2:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" ht="27.75" customHeight="1">
       <c r="B22" s="21" t="s">
         <v>45</v>
       </c>
@@ -3854,7 +3908,7 @@
       <c r="J22" s="21"/>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" ht="13.5" customHeight="1">
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -3866,11 +3920,11 @@
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -3887,12 +3941,12 @@
         <v>188</v>
       </c>
       <c r="I24" s="25"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="21" t="s">
         <v>5</v>
       </c>
@@ -3903,12 +3957,12 @@
       <c r="G25" s="21"/>
       <c r="H25" s="25"/>
       <c r="I25" s="25"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-    </row>
-    <row r="26" spans="2:11" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+    </row>
+    <row r="26" spans="2:11" ht="19.149999999999999" customHeight="1">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="21" t="s">
         <v>6</v>
       </c>
@@ -3917,12 +3971,12 @@
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-    </row>
-    <row r="27" spans="2:11" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="36"/>
-      <c r="C27" s="38" t="s">
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+    </row>
+    <row r="27" spans="2:11" ht="23.85" customHeight="1">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -3937,12 +3991,12 @@
       </c>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-    </row>
-    <row r="28" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36"/>
-      <c r="C28" s="39"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+    </row>
+    <row r="28" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="21" t="s">
         <v>5</v>
       </c>
@@ -3953,12 +4007,12 @@
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-    </row>
-    <row r="29" spans="2:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+    </row>
+    <row r="29" spans="2:11" ht="24.95" customHeight="1">
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21"/>
       <c r="E29" s="25" t="s">
         <v>80</v>
@@ -3969,12 +4023,12 @@
       </c>
       <c r="H29" s="21"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
-      <c r="C30" s="39"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="35"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="21" t="s">
         <v>6</v>
       </c>
@@ -3983,20 +4037,12 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-    </row>
-    <row r="36" ht="87.2" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+    </row>
+    <row r="36" ht="87.2" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="J4:K10"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="J24:K30"/>
@@ -4006,6 +4052,14 @@
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="J15:K20"/>
     <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="J4:K10"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4013,14 +4067,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IR36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="20" customWidth="1"/>
@@ -4033,18 +4087,18 @@
     <col min="253" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:8" ht="42" customHeight="1">
+      <c r="B1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="2:8" ht="20.25" customHeight="1">
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -4055,11 +4109,11 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:8" ht="29.25" customHeight="1">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
         <v>3</v>
@@ -4068,17 +4122,17 @@
         <v>134</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>153</v>
+        <v>192</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -4090,12 +4144,16 @@
       <c r="F4" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="39"/>
+      <c r="G4" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
@@ -4105,12 +4163,11 @@
       <c r="F5" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
-      <c r="C6" s="39"/>
+    <row r="6" spans="2:8" ht="24.75" customHeight="1">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="21" t="s">
         <v>6</v>
       </c>
@@ -4121,8 +4178,8 @@
       <c r="G6" s="2"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
+    <row r="7" spans="2:8" ht="24.75" customHeight="1">
+      <c r="B7" s="35"/>
       <c r="C7" s="27" t="s">
         <v>114</v>
       </c>
@@ -4132,9 +4189,9 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
+    <row r="8" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="38" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -4149,9 +4206,9 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+    <row r="9" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="21" t="s">
         <v>5</v>
       </c>
@@ -4162,9 +4219,9 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
     </row>
-    <row r="10" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+    <row r="10" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="21" t="s">
         <v>6</v>
       </c>
@@ -4175,7 +4232,7 @@
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="13.5" customHeight="1">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -4184,8 +4241,8 @@
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="12" spans="2:8" ht="33.75" customHeight="1">
+      <c r="B12" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -4201,8 +4258,8 @@
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="36"/>
+    <row r="13" spans="2:8" ht="33.75" customHeight="1">
+      <c r="B13" s="35"/>
       <c r="C13" s="21" t="s">
         <v>59</v>
       </c>
@@ -4214,7 +4271,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="12.75" customHeight="1">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -4223,11 +4280,11 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="38" t="s">
         <v>142</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -4237,12 +4294,12 @@
         <v>104</v>
       </c>
       <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+    <row r="16" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="21" t="s">
         <v>5</v>
       </c>
@@ -4250,12 +4307,16 @@
         <v>103</v>
       </c>
       <c r="F16" s="25"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
+      <c r="G16" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="32.25" customHeight="1">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
@@ -4263,12 +4324,16 @@
         <v>88</v>
       </c>
       <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37" t="s">
+      <c r="G17" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B18" s="35"/>
+      <c r="C18" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -4279,9 +4344,9 @@
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
     </row>
-    <row r="19" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+    <row r="19" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="21" t="s">
         <v>5</v>
       </c>
@@ -4290,9 +4355,9 @@
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
+    <row r="20" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="21" t="s">
         <v>6</v>
       </c>
@@ -4301,7 +4366,7 @@
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
     </row>
-    <row r="21" spans="2:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="11.25" customHeight="1">
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -4310,7 +4375,7 @@
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
     </row>
-    <row r="22" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="27.75" customHeight="1">
       <c r="B22" s="21" t="s">
         <v>45</v>
       </c>
@@ -4323,7 +4388,7 @@
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
     </row>
-    <row r="23" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="13.5" customHeight="1">
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -4332,11 +4397,11 @@
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -4349,9 +4414,9 @@
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
+    <row r="25" spans="2:8">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="21" t="s">
         <v>5</v>
       </c>
@@ -4362,9 +4427,9 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="2:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
+    <row r="26" spans="2:8" ht="19.149999999999999" customHeight="1">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="21" t="s">
         <v>6</v>
       </c>
@@ -4375,9 +4440,9 @@
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="2:8" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="36"/>
-      <c r="C27" s="38" t="s">
+    <row r="27" spans="2:8" ht="23.85" customHeight="1">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -4387,12 +4452,16 @@
         <v>105</v>
       </c>
       <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36"/>
-      <c r="C28" s="39"/>
+      <c r="G27" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="21" t="s">
         <v>5</v>
       </c>
@@ -4403,20 +4472,24 @@
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
+    <row r="29" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21"/>
       <c r="E29" s="25" t="s">
         <v>91</v>
       </c>
       <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
-      <c r="C30" s="39"/>
+      <c r="G29" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="35"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="21" t="s">
         <v>6</v>
       </c>
@@ -4427,14 +4500,9 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
     </row>
-    <row r="36" ht="87.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="87.2" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="C15:C17"/>
@@ -4442,6 +4510,11 @@
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4449,14 +4522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IR36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="20" customWidth="1"/>
@@ -4468,18 +4541,18 @@
     <col min="253" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:9" ht="42" customHeight="1">
+      <c r="B1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="2:9" ht="20.25" customHeight="1">
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -4488,11 +4561,11 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:9" ht="29.25" customHeight="1">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
         <v>4</v>
@@ -4508,11 +4581,11 @@
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -4524,13 +4597,17 @@
       <c r="F4" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="13"/>
+      <c r="G4" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>200</v>
+      </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="39"/>
+    <row r="5" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
@@ -4544,9 +4621,9 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
-      <c r="C6" s="39"/>
+    <row r="6" spans="2:9" ht="24.75" customHeight="1">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="21" t="s">
         <v>6</v>
       </c>
@@ -4560,8 +4637,8 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
+    <row r="7" spans="2:9" ht="24.75" customHeight="1">
+      <c r="B7" s="35"/>
       <c r="C7" s="27" t="s">
         <v>114</v>
       </c>
@@ -4572,9 +4649,9 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
+    <row r="8" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="38" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -4584,12 +4661,16 @@
         <v>106</v>
       </c>
       <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+      <c r="G8" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="21" t="s">
         <v>5</v>
       </c>
@@ -4600,9 +4681,9 @@
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
     </row>
-    <row r="10" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+    <row r="10" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="21" t="s">
         <v>6</v>
       </c>
@@ -4615,17 +4696,17 @@
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" ht="13.5" customHeight="1">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
       <c r="E11" s="25"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="12" spans="2:9" ht="33.75" customHeight="1">
+      <c r="B12" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -4639,8 +4720,8 @@
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="36"/>
+    <row r="13" spans="2:9" ht="33.75" customHeight="1">
+      <c r="B13" s="35"/>
       <c r="C13" s="21" t="s">
         <v>59</v>
       </c>
@@ -4652,7 +4733,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" ht="12.75" customHeight="1">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -4661,11 +4742,11 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="38" t="s">
         <v>142</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -4675,12 +4756,16 @@
         <v>93</v>
       </c>
       <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+      <c r="G15" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="21" t="s">
         <v>5</v>
       </c>
@@ -4691,9 +4776,9 @@
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
     </row>
-    <row r="17" spans="2:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
+    <row r="17" spans="2:8" ht="32.25" customHeight="1">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
@@ -4704,9 +4789,9 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37" t="s">
+    <row r="18" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B18" s="35"/>
+      <c r="C18" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -4719,9 +4804,9 @@
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
     </row>
-    <row r="19" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+    <row r="19" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="21" t="s">
         <v>5</v>
       </c>
@@ -4732,9 +4817,9 @@
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
+    <row r="20" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="21" t="s">
         <v>6</v>
       </c>
@@ -4743,7 +4828,7 @@
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
     </row>
-    <row r="21" spans="2:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="11.25" customHeight="1">
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -4752,7 +4837,7 @@
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
     </row>
-    <row r="22" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="27.75" customHeight="1">
       <c r="B22" s="21" t="s">
         <v>45</v>
       </c>
@@ -4765,7 +4850,7 @@
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
     </row>
-    <row r="23" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="13.5" customHeight="1">
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -4774,11 +4859,11 @@
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
     </row>
-    <row r="24" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -4791,9 +4876,9 @@
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
+    <row r="25" spans="2:8">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="21" t="s">
         <v>5</v>
       </c>
@@ -4802,9 +4887,9 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="2:8" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
+    <row r="26" spans="2:8" ht="19.149999999999999" customHeight="1">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="21" t="s">
         <v>6</v>
       </c>
@@ -4813,9 +4898,9 @@
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="2:8" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="36"/>
-      <c r="C27" s="38" t="s">
+    <row r="27" spans="2:8" ht="23.85" customHeight="1">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -4826,9 +4911,9 @@
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36"/>
-      <c r="C28" s="39"/>
+    <row r="28" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="21" t="s">
         <v>5</v>
       </c>
@@ -4837,18 +4922,18 @@
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
+    <row r="29" spans="2:8" ht="24.95" customHeight="1">
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
-      <c r="C30" s="39"/>
+    <row r="30" spans="2:8">
+      <c r="B30" s="35"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="21" t="s">
         <v>6</v>
       </c>
@@ -4857,14 +4942,9 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
     </row>
-    <row r="36" ht="87.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="87.2" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="C15:C17"/>
@@ -4872,6 +4952,11 @@
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4879,14 +4964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.875" style="20" customWidth="1"/>
     <col min="2" max="2" width="7.875" style="20" customWidth="1"/>
@@ -4897,19 +4982,19 @@
     <col min="254" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:9" ht="42" customHeight="1">
+      <c r="B1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-    </row>
-    <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="2:9" ht="20.25" customHeight="1">
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -4919,11 +5004,11 @@
       <c r="H2" s="21"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:9" ht="29.25" customHeight="1">
+      <c r="B3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
         <v>28</v>
@@ -4941,11 +5026,11 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D4" s="21" t="s">
@@ -4963,9 +5048,9 @@
       <c r="H4" s="2"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="39"/>
+    <row r="5" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
@@ -4981,9 +5066,9 @@
       <c r="H5" s="2"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
-      <c r="C6" s="39"/>
+    <row r="6" spans="2:9" ht="24.75" customHeight="1">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="21" t="s">
         <v>6</v>
       </c>
@@ -4997,8 +5082,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
+    <row r="7" spans="2:9" ht="24.75" customHeight="1">
+      <c r="B7" s="35"/>
       <c r="C7" s="27" t="s">
         <v>114</v>
       </c>
@@ -5009,9 +5094,9 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37" t="s">
+    <row r="8" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="38" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -5027,9 +5112,9 @@
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+    <row r="9" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="21" t="s">
         <v>5</v>
       </c>
@@ -5043,9 +5128,9 @@
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
+    <row r="10" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="21" t="s">
         <v>6</v>
       </c>
@@ -5055,7 +5140,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
-    <row r="11" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" ht="13.5" customHeight="1">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -5065,8 +5150,8 @@
       <c r="H11" s="21"/>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="12" spans="2:9" ht="33.75" customHeight="1">
+      <c r="B12" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -5081,8 +5166,8 @@
       <c r="H12" s="21"/>
       <c r="I12" s="25"/>
     </row>
-    <row r="13" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="36"/>
+    <row r="13" spans="2:9" ht="33.75" customHeight="1">
+      <c r="B13" s="35"/>
       <c r="C13" s="21" t="s">
         <v>59</v>
       </c>
@@ -5095,7 +5180,7 @@
       <c r="H13" s="21"/>
       <c r="I13" s="25"/>
     </row>
-    <row r="14" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" ht="12.75" customHeight="1">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -5105,11 +5190,11 @@
       <c r="H14" s="21"/>
       <c r="I14" s="25"/>
     </row>
-    <row r="15" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B15" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="38" t="s">
         <v>142</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -5125,9 +5210,9 @@
       <c r="H15" s="26"/>
       <c r="I15" s="25"/>
     </row>
-    <row r="16" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
+    <row r="16" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="21" t="s">
         <v>5</v>
       </c>
@@ -5141,9 +5226,9 @@
       <c r="H16" s="21"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
+    <row r="17" spans="2:9" ht="32.25" customHeight="1">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="21" t="s">
         <v>6</v>
       </c>
@@ -5155,9 +5240,9 @@
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
     </row>
-    <row r="18" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37" t="s">
+    <row r="18" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B18" s="35"/>
+      <c r="C18" s="38" t="s">
         <v>143</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -5171,9 +5256,9 @@
       <c r="H18" s="21"/>
       <c r="I18" s="25"/>
     </row>
-    <row r="19" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+    <row r="19" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="21" t="s">
         <v>5</v>
       </c>
@@ -5183,9 +5268,9 @@
       <c r="H19" s="21"/>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
+    <row r="20" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="21" t="s">
         <v>6</v>
       </c>
@@ -5195,7 +5280,7 @@
       <c r="H20" s="21"/>
       <c r="I20" s="25"/>
     </row>
-    <row r="21" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" ht="11.25" customHeight="1">
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -5205,7 +5290,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="2:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" ht="27.75" customHeight="1">
       <c r="B22" s="21" t="s">
         <v>45</v>
       </c>
@@ -5219,7 +5304,7 @@
       <c r="H22" s="21"/>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" ht="13.5" customHeight="1">
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -5229,11 +5314,11 @@
       <c r="H23" s="21"/>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="36" t="s">
+    <row r="24" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="38" t="s">
         <v>145</v>
       </c>
       <c r="D24" s="21" t="s">
@@ -5249,9 +5334,9 @@
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
+    <row r="25" spans="2:9">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="21" t="s">
         <v>5</v>
       </c>
@@ -5265,9 +5350,9 @@
       <c r="H25" s="25"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="2:9" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
+    <row r="26" spans="2:9" ht="19.149999999999999" customHeight="1">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="21" t="s">
         <v>6</v>
       </c>
@@ -5277,9 +5362,9 @@
       <c r="H26" s="21"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="2:9" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="36"/>
-      <c r="C27" s="38" t="s">
+    <row r="27" spans="2:9" ht="23.85" customHeight="1">
+      <c r="B27" s="35"/>
+      <c r="C27" s="36" t="s">
         <v>146</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -5295,9 +5380,9 @@
       <c r="H27" s="21"/>
       <c r="I27" s="25"/>
     </row>
-    <row r="28" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="36"/>
-      <c r="C28" s="39"/>
+    <row r="28" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="21" t="s">
         <v>5</v>
       </c>
@@ -5311,9 +5396,9 @@
       <c r="H28" s="21"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="29" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="36"/>
-      <c r="C29" s="39"/>
+    <row r="29" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
@@ -5321,9 +5406,9 @@
       <c r="H29" s="21"/>
       <c r="I29" s="25"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="36"/>
-      <c r="C30" s="39"/>
+    <row r="30" spans="2:9">
+      <c r="B30" s="35"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="21" t="s">
         <v>6</v>
       </c>
@@ -5333,14 +5418,9 @@
       <c r="H30" s="21"/>
       <c r="I30" s="25"/>
     </row>
-    <row r="36" ht="87.2" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="87.2" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="C15:C17"/>
@@ -5348,6 +5428,11 @@
     <mergeCell ref="B24:B30"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5355,14 +5440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="23.5" customWidth="1"/>
     <col min="3" max="3" width="12.875" customWidth="1"/>
@@ -5373,8 +5458,8 @@
     <col min="8" max="8" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1">
+      <c r="A1" s="54" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -5389,14 +5474,14 @@
       <c r="E1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="53"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="55"/>
       <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
@@ -5417,8 +5502,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="53"/>
+    <row r="3" spans="1:8">
+      <c r="A3" s="55"/>
       <c r="B3" s="6" t="s">
         <v>40</v>
       </c>
@@ -5433,8 +5518,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
+    <row r="4" spans="1:8">
+      <c r="A4" s="55"/>
       <c r="B4" s="6" t="s">
         <v>41</v>
       </c>
@@ -5452,9 +5537,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52" t="s">
+    <row r="5" spans="1:8" ht="7.5" customHeight="1"/>
+    <row r="6" spans="1:8" ht="30.75" customHeight="1">
+      <c r="A6" s="54" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -5470,13 +5555,13 @@
         <v>38</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="54" t="s">
+      <c r="G6" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="54"/>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
+      <c r="H6" s="56"/>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" customHeight="1">
+      <c r="A7" s="54"/>
       <c r="B7" s="6" t="s">
         <v>47</v>
       </c>
@@ -5484,8 +5569,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
+    <row r="8" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A8" s="54"/>
       <c r="B8" s="6" t="s">
         <v>48</v>
       </c>
@@ -5493,8 +5578,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
+    <row r="9" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A9" s="54"/>
       <c r="B9" s="6" t="s">
         <v>81</v>
       </c>
@@ -5502,8 +5587,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A10" s="54"/>
       <c r="B10" s="6" t="s">
         <v>82</v>
       </c>
@@ -5511,9 +5596,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
+    <row r="11" spans="1:8" ht="9.75" customHeight="1"/>
+    <row r="12" spans="1:8" ht="30.75" customHeight="1">
+      <c r="A12" s="54" t="s">
         <v>60</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -5525,11 +5610,11 @@
         <v>38</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="54"/>
       <c r="B13" s="8" t="s">
         <v>72</v>
       </c>
@@ -5538,8 +5623,8 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
+    <row r="14" spans="1:8">
+      <c r="A14" s="54"/>
       <c r="B14" s="4" t="s">
         <v>53</v>
       </c>
@@ -5547,8 +5632,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
+    <row r="15" spans="1:8">
+      <c r="A15" s="54"/>
       <c r="B15" s="4" t="s">
         <v>108</v>
       </c>
@@ -5556,8 +5641,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
+    <row r="16" spans="1:8">
+      <c r="A16" s="54"/>
       <c r="B16" s="4" t="s">
         <v>55</v>
       </c>
@@ -5565,8 +5650,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
+    <row r="17" spans="1:8">
+      <c r="A17" s="54"/>
       <c r="B17" s="4" t="s">
         <v>77</v>
       </c>
@@ -5575,8 +5660,8 @@
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52"/>
+    <row r="18" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A18" s="54"/>
       <c r="B18" s="4" t="s">
         <v>54</v>
       </c>
@@ -5585,9 +5670,9 @@
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="52" t="s">
+    <row r="19" spans="1:8" ht="8.25" customHeight="1"/>
+    <row r="20" spans="1:8" ht="30.75" customHeight="1">
+      <c r="A20" s="54" t="s">
         <v>119</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -5597,11 +5682,11 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="53"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="55"/>
       <c r="B21" s="4" t="s">
         <v>118</v>
       </c>
@@ -5609,8 +5694,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="53"/>
+    <row r="22" spans="1:8">
+      <c r="A22" s="55"/>
       <c r="B22" s="4" t="s">
         <v>120</v>
       </c>

</xml_diff>